<commit_message>
redo gorilla with updated gene ids
</commit_message>
<xml_diff>
--- a/results/modeloutput/fitness/GOPROCESS_ams.xlsx
+++ b/results/modeloutput/fitness/GOPROCESS_ams.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vistor/Documents/Work/GitHub/PhD/ms_epi_effort/results/modeloutput/fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76001AC6-D882-A346-B9A6-90B1DF3E42E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E2698CC-E501-4440-A983-6C498B5DA97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" xr2:uid="{66BDA050-FC4B-274E-B352-D60DC4BA8113}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15740" xr2:uid="{B81BC50F-43F5-9640-ABE0-FD4606DF58CD}"/>
   </bookViews>
   <sheets>
     <sheet name="GOPROCESS_ams" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>GO Term</t>
   </si>
@@ -52,13 +52,43 @@
     <t>Genes</t>
   </si>
   <si>
-    <t>GO:0001676</t>
-  </si>
-  <si>
-    <t>long-chain fatty acid metabolic process</t>
-  </si>
-  <si>
-    <t>[ACOT7  -  acyl-coa thioesterase 7, ACOT1  -  acyl-coa thioesterase 1]</t>
+    <t>GO:0030047</t>
+  </si>
+  <si>
+    <t>actin modification</t>
+  </si>
+  <si>
+    <t>[TRIM32  -  tripartite motif containing 32, TRIOBP  -  trio and f-actin binding protein]</t>
+  </si>
+  <si>
+    <t>GO:1903506</t>
+  </si>
+  <si>
+    <t>regulation of nucleic acid-templated transcription</t>
+  </si>
+  <si>
+    <t>[PSMD11  -  proteasome (prosome, macropain) 26s subunit, non-atpase, 11, TRAK1  -  trafficking protein, kinesin binding 1, CIR1  -  corepressor interacting with rbpj, 1, TCF12  -  transcription factor 12, ID1  -  inhibitor of dna binding 1, dominant negative helix-loop-helix protein, SFRP5  -  secreted frizzled-related protein 5, ZBTB7A  -  zinc finger and btb domain containing 7a, NLRC5  -  nlr family, card domain containing 5, NFKBIE  -  nuclear factor of kappa light polypeptide gene enhancer in b-cells inhibitor, epsilon, RUNX1  -  runt-related transcription factor 1, ZNF423  -  zinc finger protein 423, CBFA2T3  -  core-binding factor, runt domain, alpha subunit 2; translocated to, 3, ACVR1  -  activin a receptor, type i, NLK  -  nemo-like kinase, SPDEF  -  sam pointed domain containing ets transcription factor, GLI1  -  gli family zinc finger 1, RASL11A  -  ras-like, family 11, member a, DMRTA2  -  dmrt-like family a2, FKBP8  -  fk506 binding protein 8, 38kda, PRDM15  -  pr domain containing 15, MEF2B  -  myocyte enhancer factor 2b, HAS3  -  hyaluronan synthase 3, DOT1L  -  dot1-like histone h3k79 methyltransferase, IRF2BPL  -  interferon regulatory factor 2 binding protein-like, ZBTB39  -  zinc finger and btb domain containing 39, TSC22D3  -  tsc22 domain family, member 3, PLXND1  -  plexin d1, TBR1  -  t-box, brain, 1, TRIM32  -  tripartite motif containing 32, CXXC5  -  cxxc finger protein 5, SCMH1  -  sex comb on midleg homolog 1 (drosophila), ATXN1L  -  ataxin 1-like, BAZ1A  -  bromodomain adjacent to zinc finger domain, 1a, RNF41  -  ring finger protein 41, GATA2  -  gata binding protein 2, PPHLN1  -  periphilin 1, GAL  -  galanin/gmap prepropeptide, UBTF  -  upstream binding transcription factor, rna polymerase i, SIX4  -  six homeobox 4, NCOR2  -  nuclear receptor corepressor 2, NFIA  -  nuclear factor i/a, ELP3  -  elongator acetyltransferase complex subunit 3, DNMT3B  -  dna (cytosine-5-)-methyltransferase 3 beta, BCL11A  -  b-cell cll/lymphoma 11a (zinc finger protein), TCF3  -  transcription factor 3, HMGN1  -  high mobility group nucleosome binding domain 1, IHH  -  indian hedgehog, NFIC  -  nuclear factor i/c (ccaat-binding transcription factor)]</t>
+  </si>
+  <si>
+    <t>GO:0006355</t>
+  </si>
+  <si>
+    <t>regulation of transcription, DNA-templated</t>
+  </si>
+  <si>
+    <t>GO:2001141</t>
+  </si>
+  <si>
+    <t>regulation of RNA biosynthetic process</t>
+  </si>
+  <si>
+    <t>GO:0051252</t>
+  </si>
+  <si>
+    <t>regulation of RNA metabolic process</t>
+  </si>
+  <si>
+    <t>[TRAK1  -  trafficking protein, kinesin binding 1, SFRP5  -  secreted frizzled-related protein 5, ID1  -  inhibitor of dna binding 1, dominant negative helix-loop-helix protein, NLRC5  -  nlr family, card domain containing 5, ZNF423  -  zinc finger protein 423, NLK  -  nemo-like kinase, PCBP3  -  poly(rc) binding protein 3, FKBP8  -  fk506 binding protein 8, 38kda, DMRTA2  -  dmrt-like family a2, SRPK1  -  srsf protein kinase 1, PRDM15  -  pr domain containing 15, DOT1L  -  dot1-like histone h3k79 methyltransferase, PLXND1  -  plexin d1, TBR1  -  t-box, brain, 1, TRIM32  -  tripartite motif containing 32, CXXC5  -  cxxc finger protein 5, SCMH1  -  sex comb on midleg homolog 1 (drosophila), BAZ1A  -  bromodomain adjacent to zinc finger domain, 1a, PPHLN1  -  periphilin 1, UBTF  -  upstream binding transcription factor, rna polymerase i, SIX4  -  six homeobox 4, NFIA  -  nuclear factor i/a, ELP3  -  elongator acetyltransferase complex subunit 3, DNMT3B  -  dna (cytosine-5-)-methyltransferase 3 beta, BCL11A  -  b-cell cll/lymphoma 11a (zinc finger protein), TCF3  -  transcription factor 3, HMGN1  -  high mobility group nucleosome binding domain 1, NFIC  -  nuclear factor i/c (ccaat-binding transcription factor), PSMD11  -  proteasome (prosome, macropain) 26s subunit, non-atpase, 11, CIR1  -  corepressor interacting with rbpj, 1, TCF12  -  transcription factor 12, ZBTB7A  -  zinc finger and btb domain containing 7a, NFKBIE  -  nuclear factor of kappa light polypeptide gene enhancer in b-cells inhibitor, epsilon, RUNX1  -  runt-related transcription factor 1, CBFA2T3  -  core-binding factor, runt domain, alpha subunit 2; translocated to, 3, ACVR1  -  activin a receptor, type i, SPDEF  -  sam pointed domain containing ets transcription factor, GLI1  -  gli family zinc finger 1, RASL11A  -  ras-like, family 11, member a, MEF2B  -  myocyte enhancer factor 2b, HAS3  -  hyaluronan synthase 3, IRF2BPL  -  interferon regulatory factor 2 binding protein-like, ZBTB39  -  zinc finger and btb domain containing 39, TSC22D3  -  tsc22 domain family, member 3, ATXN1L  -  ataxin 1-like, RNF41  -  ring finger protein 41, GATA2  -  gata binding protein 2, GAL  -  galanin/gmap prepropeptide, NCOR2  -  nuclear receptor corepressor 2, CPSF7  -  cleavage and polyadenylation specific factor 7, 59kda, IHH  -  indian hedgehog]</t>
   </si>
 </sst>
 </file>
@@ -919,8 +949,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA1D6BA-CC5A-4540-BA48-F56EA49A0A8C}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95EB5D3-3295-4948-964E-DBE28D13363B}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -966,28 +996,156 @@
         <v>11</v>
       </c>
       <c r="C2" s="1">
-        <v>7.9600000000000005E-4</v>
+        <v>4.5300000000000001E-4</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>48</v>
+        <v>46.86</v>
       </c>
       <c r="F2">
-        <v>288</v>
+        <v>7404</v>
       </c>
       <c r="G2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2">
-        <v>4</v>
+        <v>158</v>
       </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.8500000000000002E-4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1.56</v>
+      </c>
+      <c r="F3">
+        <v>7404</v>
+      </c>
+      <c r="G3">
+        <v>1439</v>
+      </c>
+      <c r="H3">
+        <v>158</v>
+      </c>
+      <c r="I3">
+        <v>48</v>
+      </c>
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.8500000000000002E-4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1.56</v>
+      </c>
+      <c r="F4">
+        <v>7404</v>
+      </c>
+      <c r="G4">
+        <v>1439</v>
+      </c>
+      <c r="H4">
+        <v>158</v>
+      </c>
+      <c r="I4">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.1499999999999999E-4</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1.56</v>
+      </c>
+      <c r="F5">
+        <v>7404</v>
+      </c>
+      <c r="G5">
+        <v>1442</v>
+      </c>
+      <c r="H5">
+        <v>158</v>
+      </c>
+      <c r="I5">
+        <v>48</v>
+      </c>
+      <c r="J5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8.0800000000000002E-4</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1.51</v>
+      </c>
+      <c r="F6">
+        <v>7404</v>
+      </c>
+      <c r="G6">
+        <v>1580</v>
+      </c>
+      <c r="H6">
+        <v>158</v>
+      </c>
+      <c r="I6">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>